<commit_message>
save before upping mitochondrial content
</commit_message>
<xml_diff>
--- a/data/Granulosa_0.05_0.xlsx
+++ b/data/Granulosa_0.05_0.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -418,7 +418,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -427,13 +427,13 @@
         </is>
       </c>
       <c r="E2">
-        <v>2.27331005422854E-07</v>
+        <v>5.037683634529695E-07</v>
       </c>
       <c r="F2">
-        <v>0.0001525391046387351</v>
+        <v>0.0004564141372883903</v>
       </c>
       <c r="G2">
-        <v>9.500043068723478E-05</v>
+        <v>0.0002810497185579724</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -447,114 +447,114 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GO:0015804</t>
+          <t>GO:0030308</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>neutral amino acid transport</t>
+          <t>negative regulation of cell growth</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>5/31</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>54/28905</t>
+          <t>205/28905</t>
         </is>
       </c>
       <c r="E3">
-        <v>1.213218452189688E-05</v>
+        <v>2.498846655518077E-06</v>
       </c>
       <c r="F3">
-        <v>0.003195825119740398</v>
+        <v>0.001131977534949689</v>
       </c>
       <c r="G3">
-        <v>0.001990340532648738</v>
+        <v>0.0006970466986445163</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Rgs2/Slc38a5/Slc7a8</t>
+          <t>Map2/Grem1/Rgs2/Sema3d/Frzb</t>
         </is>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GO:0089718</t>
+          <t>GO:0045926</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>amino acid import across plasma membrane</t>
+          <t>negative regulation of growth</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>5/31</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>57/28905</t>
+          <t>261/28905</t>
         </is>
       </c>
       <c r="E4">
-        <v>1.428833883639522E-05</v>
+        <v>8.100401723483079E-06</v>
       </c>
       <c r="F4">
-        <v>0.003195825119740398</v>
+        <v>0.001917640751990751</v>
       </c>
       <c r="G4">
-        <v>0.001990340532648738</v>
+        <v>0.001180840709370394</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Rgs2/Slc38a5/Slc7a8</t>
+          <t>Map2/Grem1/Rgs2/Sema3d/Frzb</t>
         </is>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GO:1902475</t>
+          <t>GO:0009954</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>L-alpha-amino acid transmembrane transport</t>
+          <t>proximal/distal pattern formation</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>71/28905</t>
+          <t>37/28905</t>
         </is>
       </c>
       <c r="E5">
-        <v>2.769805027510257E-05</v>
+        <v>8.466405086051881E-06</v>
       </c>
       <c r="F5">
-        <v>0.004045372208010815</v>
+        <v>0.001917640751990751</v>
       </c>
       <c r="G5">
-        <v>0.002519433314895746</v>
+        <v>0.001180840709370394</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Rgs2/Slc38a5/Slc7a8</t>
+          <t>Grem1/Pbx1/Cyp26b1</t>
         </is>
       </c>
       <c r="I5">
@@ -564,188 +564,188 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GO:0015801</t>
+          <t>GO:0015804</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>aromatic amino acid transport</t>
+          <t>neutral amino acid transport</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>11/28905</t>
+          <t>54/28905</t>
         </is>
       </c>
       <c r="E6">
-        <v>3.617322391663918E-05</v>
+        <v>2.669550285318024E-05</v>
       </c>
       <c r="F6">
-        <v>0.004045372208010815</v>
+        <v>0.004544112970534627</v>
       </c>
       <c r="G6">
-        <v>0.002519433314895746</v>
+        <v>0.002798164138937321</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Slc38a5/Slc7a8</t>
+          <t>Rgs2/Slc38a5/Slc7a8</t>
         </is>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GO:0015808</t>
+          <t>GO:0089718</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>L-alanine transport</t>
+          <t>amino acid import across plasma membrane</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>11/28905</t>
+          <t>57/28905</t>
         </is>
       </c>
       <c r="E7">
-        <v>3.617322391663918E-05</v>
+        <v>3.14227894603835E-05</v>
       </c>
       <c r="F7">
-        <v>0.004045372208010815</v>
+        <v>0.004544112970534627</v>
       </c>
       <c r="G7">
-        <v>0.002519433314895746</v>
+        <v>0.002798164138937321</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Slc38a5/Slc7a8</t>
+          <t>Rgs2/Slc38a5/Slc7a8</t>
         </is>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GO:0015807</t>
+          <t>GO:0035107</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>L-amino acid transport</t>
+          <t>appendage morphogenesis</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>4/31</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>90/28905</t>
+          <t>180/28905</t>
         </is>
       </c>
       <c r="E8">
-        <v>5.634613429988482E-05</v>
+        <v>4.012461784136536E-05</v>
       </c>
       <c r="F8">
-        <v>0.005401179445031816</v>
+        <v>0.004544112970534627</v>
       </c>
       <c r="G8">
-        <v>0.003363821852188612</v>
+        <v>0.002798164138937321</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Rgs2/Slc38a5/Slc7a8</t>
+          <t>Grem1/Pcsk5/Pbx1/Cyp26b1</t>
         </is>
       </c>
       <c r="I8">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GO:1901992</t>
+          <t>GO:0035108</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>positive regulation of mitotic cell cycle phase transition</t>
+          <t>limb morphogenesis</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>4/31</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>99/28905</t>
+          <t>180/28905</t>
         </is>
       </c>
       <c r="E9">
-        <v>7.48605672202878E-05</v>
+        <v>4.012461784136536E-05</v>
       </c>
       <c r="F9">
-        <v>0.005983618691017567</v>
+        <v>0.004544112970534627</v>
       </c>
       <c r="G9">
-        <v>0.003726561487699387</v>
+        <v>0.002798164138937321</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Pbx1/Cdk1/Ube2c</t>
+          <t>Grem1/Pcsk5/Pbx1/Cyp26b1</t>
         </is>
       </c>
       <c r="I9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>GO:0003333</t>
+          <t>GO:1902475</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>amino acid transmembrane transport</t>
+          <t>L-alpha-amino acid transmembrane transport</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>102/28905</t>
+          <t>71/28905</t>
         </is>
       </c>
       <c r="E10">
-        <v>8.181483990557905E-05</v>
+        <v>6.075904345574443E-05</v>
       </c>
       <c r="F10">
-        <v>0.005983618691017567</v>
+        <v>0.005012281410397544</v>
       </c>
       <c r="G10">
-        <v>0.003726561487699387</v>
+        <v>0.003086451896724408</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -759,32 +759,32 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>GO:0032328</t>
+          <t>GO:0015801</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>alanine transport</t>
+          <t>aromatic amino acid transport</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2/24</t>
+          <t>2/31</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>17/28905</t>
+          <t>11/28905</t>
         </is>
       </c>
       <c r="E11">
-        <v>8.917464517164781E-05</v>
+        <v>6.085551381277371E-05</v>
       </c>
       <c r="F11">
-        <v>0.005983618691017567</v>
+        <v>0.005012281410397544</v>
       </c>
       <c r="G11">
-        <v>0.003726561487699387</v>
+        <v>0.003086451896724408</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -798,188 +798,188 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>GO:1901989</t>
+          <t>GO:0015808</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>positive regulation of cell cycle phase transition</t>
+          <t>L-alanine transport</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>2/31</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>119/28905</t>
+          <t>11/28905</t>
         </is>
       </c>
       <c r="E12">
-        <v>0.0001292721160025536</v>
+        <v>6.085551381277371E-05</v>
       </c>
       <c r="F12">
-        <v>0.007594023217782487</v>
+        <v>0.005012281410397544</v>
       </c>
       <c r="G12">
-        <v>0.004729511675362221</v>
+        <v>0.003086451896724408</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Pbx1/Cdk1/Ube2c</t>
+          <t>Slc38a5/Slc7a8</t>
         </is>
       </c>
       <c r="I12">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>GO:1902749</t>
+          <t>GO:0048736</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>regulation of cell cycle G2/M phase transition</t>
+          <t>appendage development</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>4/31</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>121/28905</t>
+          <t>213/28905</t>
         </is>
       </c>
       <c r="E13">
-        <v>0.0001358096551615348</v>
+        <v>7.71614678254936E-05</v>
       </c>
       <c r="F13">
-        <v>0.007594023217782487</v>
+        <v>0.0053775607576844</v>
       </c>
       <c r="G13">
-        <v>0.004729511675362221</v>
+        <v>0.003311382829758025</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Pbx1/Cdk1/Nek10</t>
+          <t>Grem1/Pcsk5/Pbx1/Cyp26b1</t>
         </is>
       </c>
       <c r="I13">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>GO:0071459</t>
+          <t>GO:0060173</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>protein localization to chromosome, centromeric region</t>
+          <t>limb development</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2/24</t>
+          <t>4/31</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>24/28905</t>
+          <t>213/28905</t>
         </is>
       </c>
       <c r="E14">
-        <v>0.0001803306529955031</v>
+        <v>7.71614678254936E-05</v>
       </c>
       <c r="F14">
-        <v>0.008799701004763599</v>
+        <v>0.0053775607576844</v>
       </c>
       <c r="G14">
-        <v>0.005480400500260646</v>
+        <v>0.003311382829758025</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Cenpa/Cdk1</t>
+          <t>Grem1/Pcsk5/Pbx1/Cyp26b1</t>
         </is>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>GO:0045931</t>
+          <t>GO:0001558</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>positive regulation of mitotic cell cycle</t>
+          <t>regulation of cell growth</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>5/31</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>134/28905</t>
+          <t>458/28905</t>
         </is>
       </c>
       <c r="E15">
-        <v>0.0001836003190263642</v>
+        <v>0.0001181737869427494</v>
       </c>
       <c r="F15">
-        <v>0.008799701004763599</v>
+        <v>0.007439944258852684</v>
       </c>
       <c r="G15">
-        <v>0.005480400500260646</v>
+        <v>0.004581352918777649</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Pbx1/Cdk1/Ube2c</t>
+          <t>Map2/Grem1/Rgs2/Sema3d/Frzb</t>
         </is>
       </c>
       <c r="I15">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GO:1905039</t>
+          <t>GO:0015807</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>carboxylic acid transmembrane transport</t>
+          <t>L-amino acid transport</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>147/28905</t>
+          <t>90/28905</t>
         </is>
       </c>
       <c r="E16">
-        <v>0.000241161310051038</v>
+        <v>0.0001231778850803425</v>
       </c>
       <c r="F16">
-        <v>0.01031733350040902</v>
+        <v>0.007439944258852684</v>
       </c>
       <c r="G16">
-        <v>0.006425572828711869</v>
+        <v>0.004581352918777649</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -993,114 +993,114 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>GO:1903825</t>
+          <t>GO:0032328</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>organic acid transmembrane transport</t>
+          <t>alanine transport</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>2/31</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>148/28905</t>
+          <t>17/28905</t>
         </is>
       </c>
       <c r="E17">
-        <v>0.0002460168941975325</v>
+        <v>0.0001498765616693205</v>
       </c>
       <c r="F17">
-        <v>0.01031733350040902</v>
+        <v>0.008486760304525272</v>
       </c>
       <c r="G17">
-        <v>0.006425572828711869</v>
+        <v>0.005225959058206569</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Rgs2/Slc38a5/Slc7a8</t>
+          <t>Slc38a5/Slc7a8</t>
         </is>
       </c>
       <c r="I17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>GO:0010971</t>
+          <t>GO:1901992</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>positive regulation of G2/M transition of mitotic cell cycle</t>
+          <t>positive regulation of mitotic cell cycle phase transition</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>29/28905</t>
+          <t>99/28905</t>
         </is>
       </c>
       <c r="E18">
-        <v>0.0002645972475906013</v>
+        <v>0.0001633860823172632</v>
       </c>
       <c r="F18">
-        <v>0.01044380900784079</v>
+        <v>0.008707517092908262</v>
       </c>
       <c r="G18">
-        <v>0.006504341008883511</v>
+        <v>0.005361896199885418</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Pbx1/Cdk1</t>
+          <t>Pbx1/Cdk1/Ube2c</t>
         </is>
       </c>
       <c r="I18">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>GO:0044839</t>
+          <t>GO:0003333</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>cell cycle G2/M phase transition</t>
+          <t>amino acid transmembrane transport</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>155/28905</t>
+          <t>102/28905</t>
         </is>
       </c>
       <c r="E19">
-        <v>0.0002817876974091216</v>
+        <v>0.0001784672611472582</v>
       </c>
       <c r="F19">
-        <v>0.01050441916452892</v>
+        <v>0.008982852144411999</v>
       </c>
       <c r="G19">
-        <v>0.006542088647451536</v>
+        <v>0.005531441427371163</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Pbx1/Cdk1/Nek10</t>
+          <t>Rgs2/Slc38a5/Slc7a8</t>
         </is>
       </c>
       <c r="I19">
@@ -1110,36 +1110,36 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>GO:1902751</t>
+          <t>GO:0046851</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>positive regulation of cell cycle G2/M phase transition</t>
+          <t>negative regulation of bone remodeling</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2/24</t>
+          <t>2/31</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>32/28905</t>
+          <t>20/28905</t>
         </is>
       </c>
       <c r="E20">
-        <v>0.000322760481382364</v>
+        <v>0.0002089668643434692</v>
       </c>
       <c r="F20">
-        <v>0.01139854121092454</v>
+        <v>0.009964419952378055</v>
       </c>
       <c r="G20">
-        <v>0.007098942443700749</v>
+        <v>0.006135869146927349</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Pbx1/Cdk1</t>
+          <t>Grem1/Ubash3b</t>
         </is>
       </c>
       <c r="I20">
@@ -1149,75 +1149,75 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>GO:0009954</t>
+          <t>GO:0048588</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>proximal/distal pattern formation</t>
+          <t>developmental cell growth</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2/24</t>
+          <t>4/31</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>37/28905</t>
+          <t>289/28905</t>
         </is>
       </c>
       <c r="E21">
-        <v>0.0004322868818422664</v>
+        <v>0.0002489226013169775</v>
       </c>
       <c r="F21">
-        <v>0.01273529978953327</v>
+        <v>0.01127619383965908</v>
       </c>
       <c r="G21">
-        <v>0.00793146759188126</v>
+        <v>0.006943630457789372</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Pbx1/Cyp26b1</t>
+          <t>S100b/Map2/Rgs2/Sema3d</t>
         </is>
       </c>
       <c r="I21">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>GO:0006865</t>
+          <t>GO:1901989</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>amino acid transport</t>
+          <t>positive regulation of cell cycle phase transition</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>180/28905</t>
+          <t>119/28905</t>
         </is>
       </c>
       <c r="E22">
-        <v>0.000436530395170291</v>
+        <v>0.0002811239180050047</v>
       </c>
       <c r="F22">
-        <v>0.01273529978953327</v>
+        <v>0.01192537893258246</v>
       </c>
       <c r="G22">
-        <v>0.00793146759188126</v>
+        <v>0.007343384261959688</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Rgs2/Slc38a5/Slc7a8</t>
+          <t>Pbx1/Cdk1/Ube2c</t>
         </is>
       </c>
       <c r="I22">
@@ -1227,36 +1227,36 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>GO:0035107</t>
+          <t>GO:1902749</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>appendage morphogenesis</t>
+          <t>regulation of cell cycle G2/M phase transition</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>180/28905</t>
+          <t>121/28905</t>
         </is>
       </c>
       <c r="E23">
-        <v>0.000436530395170291</v>
+        <v>0.0002952342849649772</v>
       </c>
       <c r="F23">
-        <v>0.01273529978953327</v>
+        <v>0.01192537893258246</v>
       </c>
       <c r="G23">
-        <v>0.00793146759188126</v>
+        <v>0.007343384261959688</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Pcsk5/Pbx1/Cyp26b1</t>
+          <t>Pbx1/Cdk1/Nek10</t>
         </is>
       </c>
       <c r="I23">
@@ -1266,192 +1266,192 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>GO:0035108</t>
+          <t>GO:0071459</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>limb morphogenesis</t>
+          <t>protein localization to chromosome, centromeric region</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>2/31</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>180/28905</t>
+          <t>24/28905</t>
         </is>
       </c>
       <c r="E24">
-        <v>0.000436530395170291</v>
+        <v>0.0003027414077807909</v>
       </c>
       <c r="F24">
-        <v>0.01273529978953327</v>
+        <v>0.01192537893258246</v>
       </c>
       <c r="G24">
-        <v>0.00793146759188126</v>
+        <v>0.007343384261959688</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Pcsk5/Pbx1/Cyp26b1</t>
+          <t>Cenpa/Cdk1</t>
         </is>
       </c>
       <c r="I24">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>GO:0006469</t>
+          <t>GO:0031954</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>negative regulation of protein kinase activity</t>
+          <t>positive regulation of protein autophosphorylation</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>2/31</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>185/28905</t>
+          <t>25/28905</t>
         </is>
       </c>
       <c r="E25">
-        <v>0.0004728549325443454</v>
+        <v>0.0003288469140865082</v>
       </c>
       <c r="F25">
-        <v>0.01322023582238566</v>
+        <v>0.01241397100676569</v>
       </c>
       <c r="G25">
-        <v>0.008233482816671278</v>
+        <v>0.007644248441484622</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Rgs2/Ubash3b/Sh3bp5</t>
+          <t>Grem1/Nek10</t>
         </is>
       </c>
       <c r="I25">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>GO:1901987</t>
+          <t>GO:0048640</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>regulation of cell cycle phase transition</t>
+          <t>negative regulation of developmental growth</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>4/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>453/28905</t>
+          <t>128/28905</t>
         </is>
       </c>
       <c r="E26">
-        <v>0.000493273206406273</v>
+        <v>0.0003482038187586517</v>
       </c>
       <c r="F26">
-        <v>0.01323945285994437</v>
+        <v>0.01261890639181354</v>
       </c>
       <c r="G26">
-        <v>0.008245451071296435</v>
+        <v>0.007770443113350964</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Pbx1/Cdk1/Nek10/Ube2c</t>
+          <t>Map2/Rgs2/Sema3d</t>
         </is>
       </c>
       <c r="I26">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>GO:0033673</t>
+          <t>GO:0010721</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>negative regulation of kinase activity</t>
+          <t>negative regulation of cell development</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>4/31</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>199/28905</t>
+          <t>326/28905</t>
         </is>
       </c>
       <c r="E27">
-        <v>0.0005847408375573375</v>
+        <v>0.0003929827623536412</v>
       </c>
       <c r="F27">
-        <v>0.01509081161542206</v>
+        <v>0.01336150263224515</v>
       </c>
       <c r="G27">
-        <v>0.009398466093532915</v>
+        <v>0.00822771743358886</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Rgs2/Ubash3b/Sh3bp5</t>
+          <t>Map2/Ubash3b/Sema3d/Frzb</t>
         </is>
       </c>
       <c r="I27">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>GO:0030308</t>
+          <t>GO:0045931</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>negative regulation of cell growth</t>
+          <t>positive regulation of mitotic cell cycle</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>205/28905</t>
+          <t>134/28905</t>
         </is>
       </c>
       <c r="E28">
-        <v>0.0006374428877510518</v>
+        <v>0.0003981904757953854</v>
       </c>
       <c r="F28">
-        <v>0.01584163621040577</v>
+        <v>0.01336150263224515</v>
       </c>
       <c r="G28">
-        <v>0.009866075104762867</v>
+        <v>0.00822771743358886</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Rgs2/Sema3d/Frzb</t>
+          <t>Pbx1/Cdk1/Ube2c</t>
         </is>
       </c>
       <c r="I28">
@@ -1461,114 +1461,114 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>GO:0098739</t>
+          <t>GO:0010971</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>import across plasma membrane</t>
+          <t>positive regulation of G2/M transition of mitotic cell cycle</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>2/31</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>209/28905</t>
+          <t>29/28905</t>
         </is>
       </c>
       <c r="E29">
-        <v>0.0006742113859760339</v>
+        <v>0.0004438516174400918</v>
       </c>
       <c r="F29">
-        <v>0.01593199798302161</v>
+        <v>0.01386653673795597</v>
       </c>
       <c r="G29">
-        <v>0.009922351869573427</v>
+        <v>0.008538706252023544</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Rgs2/Slc38a5/Slc7a8</t>
+          <t>Pbx1/Cdk1</t>
         </is>
       </c>
       <c r="I29">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>GO:0048736</t>
+          <t>GO:0034104</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>appendage development</t>
+          <t>negative regulation of tissue remodeling</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>2/31</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>213/28905</t>
+          <t>29/28905</t>
         </is>
       </c>
       <c r="E30">
-        <v>0.0007123098949189991</v>
+        <v>0.0004438516174400918</v>
       </c>
       <c r="F30">
-        <v>0.01593199798302161</v>
+        <v>0.01386653673795597</v>
       </c>
       <c r="G30">
-        <v>0.009922351869573427</v>
+        <v>0.008538706252023544</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Pcsk5/Pbx1/Cyp26b1</t>
+          <t>Grem1/Ubash3b</t>
         </is>
       </c>
       <c r="I30">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>GO:0060173</t>
+          <t>GO:0030278</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>limb development</t>
+          <t>regulation of ossification</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>213/28905</t>
+          <t>144/28905</t>
         </is>
       </c>
       <c r="E31">
-        <v>0.0007123098949189991</v>
+        <v>0.0004913601665563733</v>
       </c>
       <c r="F31">
-        <v>0.01593199798302161</v>
+        <v>0.01391163471562732</v>
       </c>
       <c r="G31">
-        <v>0.009922351869573427</v>
+        <v>0.008566476587989404</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Pcsk5/Pbx1/Cyp26b1</t>
+          <t>Mgp/Grem1/Pbx1</t>
         </is>
       </c>
       <c r="I31">
@@ -1578,75 +1578,75 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>GO:0090102</t>
+          <t>GO:0030326</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>cochlea development</t>
+          <t>embryonic limb morphogenesis</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>53/28905</t>
+          <t>144/28905</t>
         </is>
       </c>
       <c r="E32">
-        <v>0.0008872085759504023</v>
+        <v>0.0004913601665563733</v>
       </c>
       <c r="F32">
-        <v>0.01920377272460387</v>
+        <v>0.01391163471562732</v>
       </c>
       <c r="G32">
-        <v>0.01195999336680169</v>
+        <v>0.008566476587989404</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Sobp/Frzb</t>
+          <t>Grem1/Pbx1/Cyp26b1</t>
         </is>
       </c>
       <c r="I32">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>GO:0051348</t>
+          <t>GO:0035113</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>negative regulation of transferase activity</t>
+          <t>embryonic appendage morphogenesis</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>233/28905</t>
+          <t>144/28905</t>
         </is>
       </c>
       <c r="E33">
-        <v>0.0009234263055624086</v>
+        <v>0.0004913601665563733</v>
       </c>
       <c r="F33">
-        <v>0.01936309534476175</v>
+        <v>0.01391163471562732</v>
       </c>
       <c r="G33">
-        <v>0.01205921852987751</v>
+        <v>0.008566476587989404</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Rgs2/Ubash3b/Sh3bp5</t>
+          <t>Grem1/Pbx1/Cyp26b1</t>
         </is>
       </c>
       <c r="I33">
@@ -1656,75 +1656,75 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>GO:0031424</t>
+          <t>GO:1905039</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>keratinization</t>
+          <t>carboxylic acid transmembrane transport</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>60/28905</t>
+          <t>147/28905</t>
         </is>
       </c>
       <c r="E34">
-        <v>0.001135559465823388</v>
+        <v>0.0005218037270837919</v>
       </c>
       <c r="F34">
-        <v>0.0230897091384089</v>
+        <v>0.01400822870896862</v>
       </c>
       <c r="G34">
-        <v>0.01438013103450989</v>
+        <v>0.008625957030037604</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Krt79/Cyp26b1</t>
+          <t>Rgs2/Slc38a5/Slc7a8</t>
         </is>
       </c>
       <c r="I34">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>GO:0045926</t>
+          <t>GO:1903825</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>negative regulation of growth</t>
+          <t>organic acid transmembrane transport</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>261/28905</t>
+          <t>148/28905</t>
         </is>
       </c>
       <c r="E35">
-        <v>0.001280109350335759</v>
+        <v>0.0005322138941234059</v>
       </c>
       <c r="F35">
-        <v>0.02526333453162629</v>
+        <v>0.01400822870896862</v>
       </c>
       <c r="G35">
-        <v>0.01573385176728471</v>
+        <v>0.008625957030037604</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Rgs2/Sema3d/Frzb</t>
+          <t>Rgs2/Slc38a5/Slc7a8</t>
         </is>
       </c>
       <c r="I35">
@@ -1734,75 +1734,75 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>GO:0090068</t>
+          <t>GO:1902751</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>positive regulation of cell cycle process</t>
+          <t>positive regulation of cell cycle G2/M phase transition</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>2/31</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>275/28905</t>
+          <t>32/28905</t>
         </is>
       </c>
       <c r="E36">
-        <v>0.001486872216234859</v>
+        <v>0.0005411567382051894</v>
       </c>
       <c r="F36">
-        <v>0.02850546448838829</v>
+        <v>0.01400822870896862</v>
       </c>
       <c r="G36">
-        <v>0.01775303067203726</v>
+        <v>0.008625957030037604</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Pbx1/Cdk1/Ube2c</t>
+          <t>Pbx1/Cdk1</t>
         </is>
       </c>
       <c r="I36">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>GO:0055021</t>
+          <t>GO:0061037</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>regulation of cardiac muscle tissue growth</t>
+          <t>negative regulation of cartilage development</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2/24</t>
+          <t>2/31</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>85/28905</t>
+          <t>33/28905</t>
         </is>
       </c>
       <c r="E37">
-        <v>0.002261562407329312</v>
+        <v>0.000575685411276655</v>
       </c>
       <c r="F37">
-        <v>0.04152347647342776</v>
+        <v>0.01409651304369323</v>
       </c>
       <c r="G37">
-        <v>0.02586056970735088</v>
+        <v>0.008680320568325097</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Rgs2/Cdk1</t>
+          <t>Grem1/Frzb</t>
         </is>
       </c>
       <c r="I37">
@@ -1812,75 +1812,75 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>GO:0090596</t>
+          <t>GO:2001014</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>sensory organ morphogenesis</t>
+          <t>regulation of skeletal muscle cell differentiation</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>2/31</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>325/28905</t>
+          <t>33/28905</t>
         </is>
       </c>
       <c r="E38">
-        <v>0.00239252611928453</v>
+        <v>0.000575685411276655</v>
       </c>
       <c r="F38">
-        <v>0.04152347647342776</v>
+        <v>0.01409651304369323</v>
       </c>
       <c r="G38">
-        <v>0.02586056970735088</v>
+        <v>0.008680320568325097</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Sobp/Frzb/Cyp26b1</t>
+          <t>S100b/Cyp26b1</t>
         </is>
       </c>
       <c r="I38">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>GO:0001933</t>
+          <t>GO:0044839</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>negative regulation of protein phosphorylation</t>
+          <t>cell cycle G2/M phase transition</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>326/28905</t>
+          <t>155/28905</t>
         </is>
       </c>
       <c r="E39">
-        <v>0.00241343603943917</v>
+        <v>0.0006088293499853586</v>
       </c>
       <c r="F39">
-        <v>0.04152347647342776</v>
+        <v>0.01451577344965092</v>
       </c>
       <c r="G39">
-        <v>0.02586056970735088</v>
+        <v>0.008938491841890306</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Rgs2/Ubash3b/Sh3bp5</t>
+          <t>Pbx1/Cdk1/Nek10</t>
         </is>
       </c>
       <c r="I39">
@@ -1890,36 +1890,36 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>GO:0010721</t>
+          <t>GO:0030010</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>negative regulation of cell development</t>
+          <t>establishment of cell polarity</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>326/28905</t>
+          <t>170/28905</t>
         </is>
       </c>
       <c r="E40">
-        <v>0.00241343603943917</v>
+        <v>0.0007959357851519873</v>
       </c>
       <c r="F40">
-        <v>0.04152347647342776</v>
+        <v>0.01849020054737693</v>
       </c>
       <c r="G40">
-        <v>0.02586056970735088</v>
+        <v>0.01138585603591237</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Ubash3b/Sema3d/Frzb</t>
+          <t>Map2/Cenpa/Cyp26b1</t>
         </is>
       </c>
       <c r="I40">
@@ -1929,114 +1929,114 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>GO:0060420</t>
+          <t>GO:0048638</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>regulation of heart growth</t>
+          <t>regulation of developmental growth</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2/24</t>
+          <t>4/31</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>92/28905</t>
+          <t>404/28905</t>
         </is>
       </c>
       <c r="E41">
-        <v>0.002642418393807914</v>
+        <v>0.0008775861315530224</v>
       </c>
       <c r="F41">
-        <v>0.04432656855612775</v>
+        <v>0.01987732587967595</v>
       </c>
       <c r="G41">
-        <v>0.02760631848267741</v>
+        <v>0.01224001709797636</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Rgs2/Cdk1</t>
+          <t>Map2/Rgs2/Cdk1/Sema3d</t>
         </is>
       </c>
       <c r="I41">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>GO:1901990</t>
+          <t>GO:0031952</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>regulation of mitotic cell cycle phase transition</t>
+          <t>regulation of protein autophosphorylation</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>2/31</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>347/28905</t>
+          <t>42/28905</t>
         </is>
       </c>
       <c r="E42">
-        <v>0.002879119592629387</v>
+        <v>0.0009331347947893263</v>
       </c>
       <c r="F42">
-        <v>0.04674881313900445</v>
+        <v>0.02025409007763345</v>
       </c>
       <c r="G42">
-        <v>0.02911487774128914</v>
+        <v>0.01247202014772363</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Pbx1/Cdk1/Ube2c</t>
+          <t>Grem1/Nek10</t>
         </is>
       </c>
       <c r="I42">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>GO:0042326</t>
+          <t>GO:0006865</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>negative regulation of phosphorylation</t>
+          <t>amino acid transport</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>349/28905</t>
+          <t>180/28905</t>
         </is>
       </c>
       <c r="E43">
-        <v>0.002926155218834854</v>
+        <v>0.0009389313281022131</v>
       </c>
       <c r="F43">
-        <v>0.04674881313900445</v>
+        <v>0.02025409007763345</v>
       </c>
       <c r="G43">
-        <v>0.02911487774128914</v>
+        <v>0.01247202014772363</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Rgs2/Ubash3b/Sh3bp5</t>
+          <t>Rgs2/Slc38a5/Slc7a8</t>
         </is>
       </c>
       <c r="I43">
@@ -2046,75 +2046,75 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>GO:0014033</t>
+          <t>GO:0006469</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>neural crest cell differentiation</t>
+          <t>negative regulation of protein kinase activity</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>99/28905</t>
+          <t>185/28905</t>
         </is>
       </c>
       <c r="E44">
-        <v>0.00305137828764207</v>
+        <v>0.001016147587045741</v>
       </c>
       <c r="F44">
-        <v>0.04761569374436812</v>
+        <v>0.02140999334566142</v>
       </c>
       <c r="G44">
-        <v>0.02965476573302085</v>
+        <v>0.013183799782968</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Sema3d/Frzb</t>
+          <t>Rgs2/Ubash3b/Sh3bp5</t>
         </is>
       </c>
       <c r="I44">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>GO:0045787</t>
+          <t>GO:0048754</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>positive regulation of cell cycle</t>
+          <t>branching morphogenesis of an epithelial tube</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>359/28905</t>
+          <t>191/28905</t>
         </is>
       </c>
       <c r="E45">
-        <v>0.003168472609953493</v>
+        <v>0.001113983074275176</v>
       </c>
       <c r="F45">
-        <v>0.04831920730179078</v>
+        <v>0.02293792421121157</v>
       </c>
       <c r="G45">
-        <v>0.03009290971654394</v>
+        <v>0.01412466577430247</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Pbx1/Cdk1/Ube2c</t>
+          <t>Mgp/Grem1/Pbx1</t>
         </is>
       </c>
       <c r="I45">
@@ -2124,196 +2124,1561 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>GO:0033045</t>
+          <t>GO:0033673</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>regulation of sister chromatid segregation</t>
+          <t>negative regulation of kinase activity</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2/24</t>
+          <t>3/31</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>106/28905</t>
+          <t>199/28905</t>
         </is>
       </c>
       <c r="E46">
-        <v>0.003488130958188088</v>
+        <v>0.00125342865432196</v>
       </c>
       <c r="F46">
-        <v>0.04954416096781011</v>
+        <v>0.0247689588070779</v>
       </c>
       <c r="G46">
-        <v>0.03085580344218466</v>
+        <v>0.01525217633060449</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Cdk1/Ube2c</t>
+          <t>Rgs2/Ubash3b/Sh3bp5</t>
         </is>
       </c>
       <c r="I46">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>GO:0046942</t>
+          <t>GO:0030517</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>carboxylic acid transport</t>
+          <t>negative regulation of axon extension</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>2/31</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>374/28905</t>
+          <t>49/28905</t>
         </is>
       </c>
       <c r="E47">
-        <v>0.00355459177214285</v>
+        <v>0.00126858465150679</v>
       </c>
       <c r="F47">
-        <v>0.04954416096781011</v>
+        <v>0.0247689588070779</v>
       </c>
       <c r="G47">
-        <v>0.03085580344218466</v>
+        <v>0.01525217633060449</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Rgs2/Slc38a5/Slc7a8</t>
+          <t>Map2/Sema3d</t>
         </is>
       </c>
       <c r="I47">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>GO:0015849</t>
+          <t>GO:0003002</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>organic acid transport</t>
+          <t>regionalization</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>3/24</t>
+          <t>4/31</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>376/28905</t>
+          <t>448/28905</t>
         </is>
       </c>
       <c r="E48">
-        <v>0.003608156763038203</v>
+        <v>0.001286029250462541</v>
       </c>
       <c r="F48">
-        <v>0.04954416096781011</v>
+        <v>0.0247689588070779</v>
       </c>
       <c r="G48">
-        <v>0.03085580344218466</v>
+        <v>0.01525217633060449</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Rgs2/Slc38a5/Slc7a8</t>
+          <t>Grem1/Pcsk5/Pbx1/Cyp26b1</t>
         </is>
       </c>
       <c r="I48">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>GO:0010389</t>
+          <t>GO:0031400</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>regulation of G2/M transition of mitotic cell cycle</t>
+          <t>negative regulation of protein modification process</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2/24</t>
+          <t>4/31</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>108/28905</t>
+          <t>453/28905</t>
         </is>
       </c>
       <c r="E49">
-        <v>0.003617978967843063</v>
+        <v>0.001339601524886112</v>
       </c>
       <c r="F49">
-        <v>0.04954416096781011</v>
+        <v>0.0247689588070779</v>
       </c>
       <c r="G49">
-        <v>0.03085580344218466</v>
+        <v>0.01525217633060449</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Pbx1/Cdk1</t>
+          <t>Bex4/Rgs2/Ubash3b/Sh3bp5</t>
         </is>
       </c>
       <c r="I49">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>GO:0051153</t>
+          <t>GO:1901987</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>regulation of striated muscle cell differentiation</t>
+          <t>regulation of cell cycle phase transition</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2/24</t>
+          <t>4/31</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>108/28905</t>
+          <t>453/28905</t>
         </is>
       </c>
       <c r="E50">
-        <v>0.003617978967843063</v>
+        <v>0.001339601524886112</v>
       </c>
       <c r="F50">
-        <v>0.04954416096781011</v>
+        <v>0.0247689588070779</v>
       </c>
       <c r="G50">
-        <v>0.03085580344218466</v>
+        <v>0.01525217633060449</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Rgs2/Cyp26b1</t>
+          <t>Pbx1/Cdk1/Nek10/Ube2c</t>
         </is>
       </c>
       <c r="I50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>GO:1990138</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>neuron projection extension</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>3/31</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>208/28905</t>
+        </is>
+      </c>
+      <c r="E51">
+        <v>0.001422943187683337</v>
+      </c>
+      <c r="F51">
+        <v>0.02562774601212033</v>
+      </c>
+      <c r="G51">
+        <v>0.01578099847382802</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>S100b/Map2/Sema3d</t>
+        </is>
+      </c>
+      <c r="I51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>GO:0098739</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>import across plasma membrane</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>3/31</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>209/28905</t>
+        </is>
+      </c>
+      <c r="E52">
+        <v>0.001442621464258429</v>
+      </c>
+      <c r="F52">
+        <v>0.02562774601212033</v>
+      </c>
+      <c r="G52">
+        <v>0.01578099847382802</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Rgs2/Slc38a5/Slc7a8</t>
+        </is>
+      </c>
+      <c r="I52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>GO:0090102</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>cochlea development</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2/31</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>53/28905</t>
+        </is>
+      </c>
+      <c r="E53">
+        <v>0.001482525721127522</v>
+      </c>
+      <c r="F53">
+        <v>0.0258301596796449</v>
+      </c>
+      <c r="G53">
+        <v>0.01590564032788637</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Sobp/Frzb</t>
+        </is>
+      </c>
+      <c r="I53">
         <v>2</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>GO:0007519</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>skeletal muscle tissue development</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>3/31</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>218/28905</t>
+        </is>
+      </c>
+      <c r="E54">
+        <v>0.001627476040833898</v>
+      </c>
+      <c r="F54">
+        <v>0.02782062816972663</v>
+      </c>
+      <c r="G54">
+        <v>0.01713132674561998</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>S100b/Meg3/Cyp26b1</t>
+        </is>
+      </c>
+      <c r="I54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>GO:0051216</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>cartilage development</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>3/31</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>224/28905</t>
+        </is>
+      </c>
+      <c r="E55">
+        <v>0.00175859412498944</v>
+      </c>
+      <c r="F55">
+        <v>0.02910597951493432</v>
+      </c>
+      <c r="G55">
+        <v>0.01792281764019425</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Mgp/Grem1/Frzb</t>
+        </is>
+      </c>
+      <c r="I55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>GO:0050922</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>negative regulation of chemotaxis</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>2/31</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>58/28905</t>
+        </is>
+      </c>
+      <c r="E56">
+        <v>0.001772463773921838</v>
+      </c>
+      <c r="F56">
+        <v>0.02910597951493432</v>
+      </c>
+      <c r="G56">
+        <v>0.01792281764019425</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Grem1/Sema3d</t>
+        </is>
+      </c>
+      <c r="I56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>GO:0007389</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>pattern specification process</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>4/31</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>491/28905</t>
+        </is>
+      </c>
+      <c r="E57">
+        <v>0.001799045091430819</v>
+      </c>
+      <c r="F57">
+        <v>0.02910597951493432</v>
+      </c>
+      <c r="G57">
+        <v>0.01792281764019425</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Grem1/Pcsk5/Pbx1/Cyp26b1</t>
+        </is>
+      </c>
+      <c r="I57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>GO:0061138</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>morphogenesis of a branching epithelium</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>3/31</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>229/28905</t>
+        </is>
+      </c>
+      <c r="E58">
+        <v>0.001872774275981817</v>
+      </c>
+      <c r="F58">
+        <v>0.02911719400056816</v>
+      </c>
+      <c r="G58">
+        <v>0.01792972327210541</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Mgp/Grem1/Pbx1</t>
+        </is>
+      </c>
+      <c r="I58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>GO:0031424</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>keratinization</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>2/31</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>60/28905</t>
+        </is>
+      </c>
+      <c r="E59">
+        <v>0.001895389620956849</v>
+      </c>
+      <c r="F59">
+        <v>0.02911719400056816</v>
+      </c>
+      <c r="G59">
+        <v>0.01792972327210541</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Krt79/Cyp26b1</t>
+        </is>
+      </c>
+      <c r="I59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>GO:0060538</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>skeletal muscle organ development</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>3/31</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>230/28905</t>
+        </is>
+      </c>
+      <c r="E60">
+        <v>0.001896152810191524</v>
+      </c>
+      <c r="F60">
+        <v>0.02911719400056816</v>
+      </c>
+      <c r="G60">
+        <v>0.01792972327210541</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>S100b/Meg3/Cyp26b1</t>
+        </is>
+      </c>
+      <c r="I60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>GO:0051348</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>negative regulation of transferase activity</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>3/31</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>233/28905</t>
+        </is>
+      </c>
+      <c r="E61">
+        <v>0.001967382749776581</v>
+      </c>
+      <c r="F61">
+        <v>0.02970747952162638</v>
+      </c>
+      <c r="G61">
+        <v>0.01829320802423839</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Rgs2/Ubash3b/Sh3bp5</t>
+        </is>
+      </c>
+      <c r="I61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>GO:0007163</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>establishment or maintenance of cell polarity</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>3/31</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>240/28905</t>
+        </is>
+      </c>
+      <c r="E62">
+        <v>0.002140035022656992</v>
+      </c>
+      <c r="F62">
+        <v>0.0314625492494259</v>
+      </c>
+      <c r="G62">
+        <v>0.01937394109700909</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Map2/Cenpa/Cyp26b1</t>
+        </is>
+      </c>
+      <c r="I62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>GO:0046850</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>regulation of bone remodeling</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>2/31</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>64/28905</t>
+        </is>
+      </c>
+      <c r="E63">
+        <v>0.002153066284177048</v>
+      </c>
+      <c r="F63">
+        <v>0.0314625492494259</v>
+      </c>
+      <c r="G63">
+        <v>0.01937394109700909</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Grem1/Ubash3b</t>
+        </is>
+      </c>
+      <c r="I63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>GO:0001658</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>branching involved in ureteric bud morphogenesis</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>2/31</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>67/28905</t>
+        </is>
+      </c>
+      <c r="E64">
+        <v>0.002356606251557899</v>
+      </c>
+      <c r="F64">
+        <v>0.03362832865062081</v>
+      </c>
+      <c r="G64">
+        <v>0.02070758009158712</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Grem1/Pbx1</t>
+        </is>
+      </c>
+      <c r="I64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>GO:0001763</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>morphogenesis of a branching structure</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>3/31</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>249/28905</t>
+        </is>
+      </c>
+      <c r="E65">
+        <v>0.002375511074657541</v>
+      </c>
+      <c r="F65">
+        <v>0.03362832865062081</v>
+      </c>
+      <c r="G65">
+        <v>0.02070758009158712</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Mgp/Grem1/Pbx1</t>
+        </is>
+      </c>
+      <c r="I65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>GO:0030323</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>respiratory tube development</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>3/31</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>251/28905</t>
+        </is>
+      </c>
+      <c r="E66">
+        <v>0.002429933033118389</v>
+      </c>
+      <c r="F66">
+        <v>0.03386952812315785</v>
+      </c>
+      <c r="G66">
+        <v>0.02085610538546957</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Mgp/Meg3/Pcsk5</t>
+        </is>
+      </c>
+      <c r="I66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>GO:0048762</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>mesenchymal cell differentiation</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>3/31</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>254/28905</t>
+        </is>
+      </c>
+      <c r="E67">
+        <v>0.002513010409446955</v>
+      </c>
+      <c r="F67">
+        <v>0.03449677925695365</v>
+      </c>
+      <c r="G67">
+        <v>0.02124235274333151</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Grem1/Sema3d/Frzb</t>
+        </is>
+      </c>
+      <c r="I67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>GO:0050771</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>negative regulation of axonogenesis</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>2/31</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>71/28905</t>
+        </is>
+      </c>
+      <c r="E68">
+        <v>0.002641598423460066</v>
+      </c>
+      <c r="F68">
+        <v>0.03572071897992268</v>
+      </c>
+      <c r="G68">
+        <v>0.02199602772087722</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Map2/Sema3d</t>
+        </is>
+      </c>
+      <c r="I68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>GO:0061035</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>regulation of cartilage development</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>2/31</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>73/28905</t>
+        </is>
+      </c>
+      <c r="E69">
+        <v>0.002789889022199182</v>
+      </c>
+      <c r="F69">
+        <v>0.03717116844283028</v>
+      </c>
+      <c r="G69">
+        <v>0.02288918238027193</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Grem1/Frzb</t>
+        </is>
+      </c>
+      <c r="I69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>GO:0060675</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>ureteric bud morphogenesis</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>2/31</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>74/28905</t>
+        </is>
+      </c>
+      <c r="E70">
+        <v>0.002865475890950851</v>
+      </c>
+      <c r="F70">
+        <v>0.03762494430726769</v>
+      </c>
+      <c r="G70">
+        <v>0.0231686075088322</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Grem1/Pbx1</t>
+        </is>
+      </c>
+      <c r="I70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>GO:0090068</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>positive regulation of cell cycle process</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>3/31</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>275/28905</t>
+        </is>
+      </c>
+      <c r="E71">
+        <v>0.003144092445602977</v>
+      </c>
+      <c r="F71">
+        <v>0.0405452476920148</v>
+      </c>
+      <c r="G71">
+        <v>0.02496686566372469</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Pbx1/Cdk1/Ube2c</t>
+        </is>
+      </c>
+      <c r="I71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>GO:0072171</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>mesonephric tubule morphogenesis</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>2/31</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>78/28905</t>
+        </is>
+      </c>
+      <c r="E72">
+        <v>0.003177386960411756</v>
+      </c>
+      <c r="F72">
+        <v>0.0405452476920148</v>
+      </c>
+      <c r="G72">
+        <v>0.02496686566372469</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Grem1/Pbx1</t>
+        </is>
+      </c>
+      <c r="I72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>GO:0048738</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>cardiac muscle tissue development</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>3/31</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>280/28905</t>
+        </is>
+      </c>
+      <c r="E73">
+        <v>0.003307408670779856</v>
+      </c>
+      <c r="F73">
+        <v>0.04161822577397985</v>
+      </c>
+      <c r="G73">
+        <v>0.02562758180575034</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Grem1/Rgs2/Cdk1</t>
+        </is>
+      </c>
+      <c r="I73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>GO:0048863</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>stem cell differentiation</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>3/31</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>284/28905</t>
+        </is>
+      </c>
+      <c r="E74">
+        <v>0.003441755336024525</v>
+      </c>
+      <c r="F74">
+        <v>0.04271548403340027</v>
+      </c>
+      <c r="G74">
+        <v>0.02630324914337416</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Grem1/Sema3d/Frzb</t>
+        </is>
+      </c>
+      <c r="I74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>GO:0060560</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>developmental growth involved in morphogenesis</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>3/31</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>290/28905</t>
+        </is>
+      </c>
+      <c r="E75">
+        <v>0.003649493479365938</v>
+      </c>
+      <c r="F75">
+        <v>0.04468163638250729</v>
+      </c>
+      <c r="G75">
+        <v>0.0275139622199708</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>S100b/Map2/Sema3d</t>
+        </is>
+      </c>
+      <c r="I75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>GO:0055021</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>regulation of cardiac muscle tissue growth</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>2/31</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>85/28905</t>
+        </is>
+      </c>
+      <c r="E76">
+        <v>0.00375974343562153</v>
+      </c>
+      <c r="F76">
+        <v>0.04541770070230809</v>
+      </c>
+      <c r="G76">
+        <v>0.02796721432813208</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Rgs2/Cdk1</t>
+        </is>
+      </c>
+      <c r="I76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>GO:0072078</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>nephron tubule morphogenesis</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>2/31</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>86/28905</t>
+        </is>
+      </c>
+      <c r="E77">
+        <v>0.003846698863884094</v>
+      </c>
+      <c r="F77">
+        <v>0.04585669961419722</v>
+      </c>
+      <c r="G77">
+        <v>0.02823754013654529</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Grem1/Pbx1</t>
+        </is>
+      </c>
+      <c r="I77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>GO:0034103</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>regulation of tissue remodeling</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>2/31</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>87/28905</t>
+        </is>
+      </c>
+      <c r="E78">
+        <v>0.003934588766196261</v>
+      </c>
+      <c r="F78">
+        <v>0.04586612893384787</v>
+      </c>
+      <c r="G78">
+        <v>0.02824334650277608</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Grem1/Ubash3b</t>
+        </is>
+      </c>
+      <c r="I78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>GO:0030500</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>regulation of bone mineralization</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>2/31</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>88/28905</t>
+        </is>
+      </c>
+      <c r="E79">
+        <v>0.004023411170716064</v>
+      </c>
+      <c r="F79">
+        <v>0.04586612893384787</v>
+      </c>
+      <c r="G79">
+        <v>0.02824334650277608</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Mgp/Grem1</t>
+        </is>
+      </c>
+      <c r="I79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>GO:0072088</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>nephron epithelium morphogenesis</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>2/31</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>88/28905</t>
+        </is>
+      </c>
+      <c r="E80">
+        <v>0.004023411170716064</v>
+      </c>
+      <c r="F80">
+        <v>0.04586612893384787</v>
+      </c>
+      <c r="G80">
+        <v>0.02824334650277608</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Grem1/Pbx1</t>
+        </is>
+      </c>
+      <c r="I80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>GO:0014706</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>striated muscle tissue development</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>3/31</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>301/28905</t>
+        </is>
+      </c>
+      <c r="E81">
+        <v>0.004049989309832042</v>
+      </c>
+      <c r="F81">
+        <v>0.04586612893384787</v>
+      </c>
+      <c r="G81">
+        <v>0.02824334650277608</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Grem1/Rgs2/Cdk1</t>
+        </is>
+      </c>
+      <c r="I81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>GO:0072028</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>nephron morphogenesis</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>2/31</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>90/28905</t>
+        </is>
+      </c>
+      <c r="E82">
+        <v>0.004203845613597873</v>
+      </c>
+      <c r="F82">
+        <v>0.04702079167802066</v>
+      </c>
+      <c r="G82">
+        <v>0.02895436225090153</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Grem1/Pbx1</t>
+        </is>
+      </c>
+      <c r="I82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>GO:0060420</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>regulation of heart growth</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>2/31</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>92/28905</t>
+        </is>
+      </c>
+      <c r="E83">
+        <v>0.004387986476090958</v>
+      </c>
+      <c r="F83">
+        <v>0.04789778008841456</v>
+      </c>
+      <c r="G83">
+        <v>0.02949439229331906</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Rgs2/Cdk1</t>
+        </is>
+      </c>
+      <c r="I83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>GO:0061333</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>renal tubule morphogenesis</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>2/31</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>92/28905</t>
+        </is>
+      </c>
+      <c r="E84">
+        <v>0.004387986476090958</v>
+      </c>
+      <c r="F84">
+        <v>0.04789778008841456</v>
+      </c>
+      <c r="G84">
+        <v>0.02949439229331906</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Grem1/Pbx1</t>
+        </is>
+      </c>
+      <c r="I84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>GO:0060485</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>mesenchyme development</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>3/31</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>314/28905</t>
+        </is>
+      </c>
+      <c r="E85">
+        <v>0.004556677187952464</v>
+      </c>
+      <c r="F85">
+        <v>0.04914701824148729</v>
+      </c>
+      <c r="G85">
+        <v>0.03026364548389482</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Grem1/Sema3d/Frzb</t>
+        </is>
+      </c>
+      <c r="I85">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>